<commit_message>
Sala Covid_45 - pediente secuenciamiento
</commit_message>
<xml_diff>
--- a/Lista_programas_inputs_outputs.xlsx
+++ b/Lista_programas_inputs_outputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\DIRESA_covid_cusco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\GERESA_covid_cusco\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C03090-43DB-45C6-A611-F264CE6725C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,24 +18,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$141</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="276">
   <si>
     <t>Programa</t>
   </si>
@@ -882,11 +876,14 @@
   <si>
     <t>2e_series_semanales_provincias.do</t>
   </si>
+  <si>
+    <t>datos_secuenciamiento_netlab.dta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1322,14 +1319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:XFD139"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A82" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2253,7 @@
         <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>164</v>
+        <v>275</v>
       </c>
       <c r="E96" t="s">
         <v>225</v>

</xml_diff>